<commit_message>
finished resytling old RSM executions
</commit_message>
<xml_diff>
--- a/ProbenSpreadsheet.xlsx
+++ b/ProbenSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdcj\Documents\_MasterThesis\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB28A5B5-AB7B-4C0D-967E-380080D3497A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B3D8D4-0967-455F-BC01-D2BBAC456379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51720" yWindow="7155" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51720" yWindow="4785" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Probenübersicht" sheetId="1" r:id="rId1"/>
@@ -2634,8 +2634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P179" sqref="P179"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
data for new RSM's and plotting done
</commit_message>
<xml_diff>
--- a/ProbenSpreadsheet.xlsx
+++ b/ProbenSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdcj\Documents\_MasterThesis\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B3D8D4-0967-455F-BC01-D2BBAC456379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38E4328-97FE-42FB-B954-4F976B8CDD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51720" yWindow="4785" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51720" yWindow="7155" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Probenübersicht" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="316">
   <si>
     <t>Id</t>
   </si>
@@ -2634,9 +2634,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P179" sqref="P179"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W175" sqref="W175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -12301,7 +12301,9 @@
         <v>144</v>
       </c>
       <c r="AB171" s="255"/>
-      <c r="AC171" s="255"/>
+      <c r="AC171" s="255" t="s">
+        <v>144</v>
+      </c>
       <c r="AD171" s="21"/>
     </row>
     <row r="172" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -12414,7 +12416,7 @@
       </c>
       <c r="AB173" s="255"/>
       <c r="AC173" s="255" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="AD173" s="21"/>
     </row>
@@ -12981,7 +12983,9 @@
         <v>144</v>
       </c>
       <c r="AB183" s="258"/>
-      <c r="AC183" s="258"/>
+      <c r="AC183" s="258" t="s">
+        <v>144</v>
+      </c>
       <c r="AD183" s="25"/>
     </row>
     <row r="184" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -13207,7 +13211,9 @@
         <v>144</v>
       </c>
       <c r="AB187" s="255"/>
-      <c r="AC187" s="255"/>
+      <c r="AC187" s="255" t="s">
+        <v>144</v>
+      </c>
       <c r="AD187" s="21"/>
     </row>
     <row r="188" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -13321,7 +13327,7 @@
       </c>
       <c r="AB189" s="255"/>
       <c r="AC189" s="255" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="AD189" s="21"/>
     </row>
@@ -13435,7 +13441,9 @@
         <v>144</v>
       </c>
       <c r="AB191" s="258"/>
-      <c r="AC191" s="258"/>
+      <c r="AC191" s="258" t="s">
+        <v>144</v>
+      </c>
       <c r="AD191" s="25"/>
     </row>
     <row r="192" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -13549,7 +13557,7 @@
       </c>
       <c r="AB193" s="258"/>
       <c r="AC193" s="258" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="AD193" s="25"/>
     </row>

</xml_diff>

<commit_message>
- added lots of data files (mainly RSM stuff) - RSM analysis for Sofie - 2d gauss fit downloaded but abandoned - changes in RSM analysis - script for strain for pseudomorphic growth - peaks.txt file now can be read with "shape left" as Lorentz
</commit_message>
<xml_diff>
--- a/ProbenSpreadsheet.xlsx
+++ b/ProbenSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdcj\Documents\_MasterThesis\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38E4328-97FE-42FB-B954-4F976B8CDD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AC632A-C9B9-4812-8DCA-846C2FB81719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51720" yWindow="7155" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48" yWindow="-48" windowWidth="20832" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Probenübersicht" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="316">
   <si>
     <t>Id</t>
   </si>
@@ -2634,9 +2634,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W175" sqref="W175"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H202" sqref="H202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -12359,7 +12359,9 @@
         <v>144</v>
       </c>
       <c r="AB172" s="255"/>
-      <c r="AC172" s="255"/>
+      <c r="AC172" s="255" t="s">
+        <v>130</v>
+      </c>
       <c r="AD172" s="21"/>
     </row>
     <row r="173" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -13269,7 +13271,9 @@
         <v>144</v>
       </c>
       <c r="AB188" s="255"/>
-      <c r="AC188" s="255"/>
+      <c r="AC188" s="255" t="s">
+        <v>130</v>
+      </c>
       <c r="AD188" s="21"/>
     </row>
     <row r="189" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -13377,8 +13381,8 @@
       <c r="V190" s="27"/>
       <c r="W190" s="27"/>
       <c r="X190" s="27"/>
-      <c r="Y190" s="13" t="s">
-        <v>130</v>
+      <c r="Y190" s="20" t="s">
+        <v>144</v>
       </c>
       <c r="Z190" s="258"/>
       <c r="AA190" s="20" t="s">
@@ -13433,8 +13437,8 @@
       <c r="V191" s="27"/>
       <c r="W191" s="27"/>
       <c r="X191" s="27"/>
-      <c r="Y191" s="13" t="s">
-        <v>130</v>
+      <c r="Y191" s="20" t="s">
+        <v>144</v>
       </c>
       <c r="Z191" s="258"/>
       <c r="AA191" s="20" t="s">
@@ -13492,15 +13496,17 @@
       <c r="V192" s="27"/>
       <c r="W192" s="27"/>
       <c r="X192" s="27"/>
-      <c r="Y192" s="13" t="s">
-        <v>130</v>
+      <c r="Y192" s="20" t="s">
+        <v>144</v>
       </c>
       <c r="Z192" s="258"/>
       <c r="AA192" s="20" t="s">
         <v>144</v>
       </c>
       <c r="AB192" s="258"/>
-      <c r="AC192" s="258"/>
+      <c r="AC192" s="258" t="s">
+        <v>130</v>
+      </c>
       <c r="AD192" s="25"/>
     </row>
     <row r="193" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -13548,8 +13554,8 @@
       <c r="V193" s="27"/>
       <c r="W193" s="27"/>
       <c r="X193" s="27"/>
-      <c r="Y193" s="13" t="s">
-        <v>130</v>
+      <c r="Y193" s="20" t="s">
+        <v>144</v>
       </c>
       <c r="Z193" s="258"/>
       <c r="AA193" s="20" t="s">

</xml_diff>

<commit_message>
Finished tilt and shear correction; implemented m-plane RSM analysis
</commit_message>
<xml_diff>
--- a/ProbenSpreadsheet.xlsx
+++ b/ProbenSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdcj\Documents\_MasterThesis\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AC632A-C9B9-4812-8DCA-846C2FB81719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A5B9F7-5681-49B4-800C-FFB7B7EC7EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="-48" windowWidth="20832" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51720" yWindow="7155" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Probenübersicht" sheetId="1" r:id="rId1"/>
@@ -2634,9 +2634,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H202" sqref="H202"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L115" sqref="L115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
added peak data for r- and c-RSM's; completed r-plane RSM analysis script
</commit_message>
<xml_diff>
--- a/ProbenSpreadsheet.xlsx
+++ b/ProbenSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdcj\Documents\_MasterThesis\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A5B9F7-5681-49B4-800C-FFB7B7EC7EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01B8D85-9501-4F68-A8E2-4F56AB5A1738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51720" yWindow="7155" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51720" yWindow="4785" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Probenübersicht" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="318">
   <si>
     <t>Id</t>
   </si>
@@ -982,6 +982,12 @@
   </si>
   <si>
     <t>W6933</t>
+  </si>
+  <si>
+    <t>RSM with longer integration time needed</t>
+  </si>
+  <si>
+    <t>RSM with other range needed (reflection not visible)</t>
   </si>
 </sst>
 </file>
@@ -1955,7 +1961,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="296">
+  <cellXfs count="297">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -2276,6 +2282,7 @@
     <xf numFmtId="164" fontId="0" fillId="35" borderId="14" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="35" borderId="14" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="59" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2635,8 +2642,8 @@
   <dimension ref="A1:AD193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L115" sqref="L115"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -9603,7 +9610,9 @@
       <c r="C125" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="D125" s="21"/>
+      <c r="D125" s="296" t="s">
+        <v>316</v>
+      </c>
       <c r="E125" s="21" t="s">
         <v>49</v>
       </c>
@@ -9842,7 +9851,9 @@
       <c r="C129" s="168" t="s">
         <v>258</v>
       </c>
-      <c r="D129" s="168"/>
+      <c r="D129" s="296" t="s">
+        <v>317</v>
+      </c>
       <c r="E129" s="168" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
1) some new plot features; 2) c-plane graphics for TCO poster
</commit_message>
<xml_diff>
--- a/ProbenSpreadsheet.xlsx
+++ b/ProbenSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdcj\Documents\_MasterThesis\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01B8D85-9501-4F68-A8E2-4F56AB5A1738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0203C44-52A5-4608-A9CD-B4BE172DEA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51720" yWindow="4785" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="318">
   <si>
     <t>Id</t>
   </si>
@@ -1961,7 +1961,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="297">
+  <cellXfs count="299">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -2283,6 +2283,8 @@
     <xf numFmtId="1" fontId="0" fillId="35" borderId="14" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="59" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="16" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="37" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2642,8 +2644,8 @@
   <dimension ref="A1:AD193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F125" sqref="F125"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S133" sqref="S133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -9664,7 +9666,9 @@
         <v>144</v>
       </c>
       <c r="AB125" s="255"/>
-      <c r="AC125" s="255"/>
+      <c r="AC125" s="298" t="s">
+        <v>144</v>
+      </c>
       <c r="AD125" s="21"/>
     </row>
     <row r="126" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -9899,7 +9903,9 @@
         <v>144</v>
       </c>
       <c r="AB129" s="257"/>
-      <c r="AC129" s="257"/>
+      <c r="AC129" s="297" t="s">
+        <v>144</v>
+      </c>
       <c r="AD129" s="168"/>
     </row>
     <row r="130" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -10357,7 +10363,9 @@
         <v>144</v>
       </c>
       <c r="AB137" s="257"/>
-      <c r="AC137" s="257"/>
+      <c r="AC137" s="297" t="s">
+        <v>144</v>
+      </c>
       <c r="AD137" s="168"/>
     </row>
     <row r="138" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -10814,7 +10822,9 @@
         <v>144</v>
       </c>
       <c r="AB145" s="257"/>
-      <c r="AC145" s="257"/>
+      <c r="AC145" s="297" t="s">
+        <v>144</v>
+      </c>
       <c r="AD145" s="168"/>
     </row>
     <row r="146" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -11761,7 +11771,9 @@
         <v>144</v>
       </c>
       <c r="AB161" s="257"/>
-      <c r="AC161" s="257"/>
+      <c r="AC161" s="297" t="s">
+        <v>144</v>
+      </c>
       <c r="AD161" s="168"/>
     </row>
     <row r="162" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
scripts for TCO: r- and c-plane
</commit_message>
<xml_diff>
--- a/ProbenSpreadsheet.xlsx
+++ b/ProbenSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdcj\Documents\_MasterThesis\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0203C44-52A5-4608-A9CD-B4BE172DEA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3880D0A7-8A5D-4C39-87EC-87B18F822CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51720" yWindow="4785" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="318">
   <si>
     <t>Id</t>
   </si>
@@ -2644,8 +2644,8 @@
   <dimension ref="A1:AD193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S133" sqref="S133"/>
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC184" sqref="AC184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -12383,7 +12383,7 @@
       </c>
       <c r="AB172" s="255"/>
       <c r="AC172" s="255" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="AD172" s="21"/>
     </row>
@@ -13066,7 +13066,9 @@
         <v>144</v>
       </c>
       <c r="AB184" s="258"/>
-      <c r="AC184" s="258"/>
+      <c r="AC184" s="258" t="s">
+        <v>144</v>
+      </c>
       <c r="AD184" s="25"/>
     </row>
     <row r="185" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -13295,7 +13297,7 @@
       </c>
       <c r="AB188" s="255"/>
       <c r="AC188" s="255" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="AD188" s="21"/>
     </row>
@@ -13528,7 +13530,7 @@
       </c>
       <c r="AB192" s="258"/>
       <c r="AC192" s="258" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="AD192" s="25"/>
     </row>

</xml_diff>

<commit_message>
m-evaluation for TCO finished
</commit_message>
<xml_diff>
--- a/ProbenSpreadsheet.xlsx
+++ b/ProbenSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdcj\Documents\_MasterThesis\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3880D0A7-8A5D-4C39-87EC-87B18F822CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666CC3C9-0DB3-4739-B5FD-D70D20352458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51720" yWindow="4785" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2645,7 +2645,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC184" sqref="AC184"/>
+      <selection pane="bottomLeft" activeCell="AC192" sqref="AC192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
moved stuff to .archive/ which is not under source control; added data for buffer layers
</commit_message>
<xml_diff>
--- a/ProbenSpreadsheet.xlsx
+++ b/ProbenSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdcj\Documents\_MasterThesis\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666CC3C9-0DB3-4739-B5FD-D70D20352458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED77A226-59B1-41A4-AA68-B2FEF5878F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51720" yWindow="4785" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48" yWindow="-48" windowWidth="20832" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Probenübersicht" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1817" uniqueCount="331">
   <si>
     <t>Id</t>
   </si>
@@ -988,6 +988,45 @@
   </si>
   <si>
     <t>RSM with other range needed (reflection not visible)</t>
+  </si>
+  <si>
+    <t>W6957c</t>
+  </si>
+  <si>
+    <t>W6957m</t>
+  </si>
+  <si>
+    <t>W6957r</t>
+  </si>
+  <si>
+    <t>W6957a</t>
+  </si>
+  <si>
+    <t>W6959c</t>
+  </si>
+  <si>
+    <t>W6959m</t>
+  </si>
+  <si>
+    <t>W6959r</t>
+  </si>
+  <si>
+    <t>W6959a</t>
+  </si>
+  <si>
+    <t>W6957</t>
+  </si>
+  <si>
+    <t>W6959</t>
+  </si>
+  <si>
+    <t>Cr2O3_buffer</t>
+  </si>
+  <si>
+    <t>ex-situ</t>
+  </si>
+  <si>
+    <t>in-situ</t>
   </si>
 </sst>
 </file>
@@ -1961,7 +2000,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="299">
+  <cellXfs count="361">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -2285,6 +2324,68 @@
     <xf numFmtId="49" fontId="16" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="37" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="44" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="15" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="50" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="40" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="40" borderId="18" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="40" borderId="18" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="40" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="46" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="40" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="52" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="40" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="40" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="39" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="39" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="39" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="39" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="39" borderId="30" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="39" borderId="30" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="39" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="45" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="39" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="58" borderId="31" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="51" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="39" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="37" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="39" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="39" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="58" borderId="24" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="59" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="47" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="53" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="40" borderId="30" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="40" borderId="30" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="33" borderId="14" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="19" fillId="33" borderId="14" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="33" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="43" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="19" fillId="33" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="19" fillId="33" borderId="15" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="49" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="55" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="33" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="19" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="23" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="30" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2641,11 +2742,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD193"/>
+  <dimension ref="A1:AD203"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC192" sqref="AC192"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J194" sqref="J194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -2675,7 +2776,7 @@
     <col min="31" max="16384" width="8.83984375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="49" customFormat="1" ht="57.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:30" s="49" customFormat="1" ht="57.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -3140,107 +3241,107 @@
       <c r="AD11" s="32"/>
     </row>
     <row r="12" spans="1:30" s="35" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="344" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32" t="s">
+      <c r="B12" s="344"/>
+      <c r="C12" s="344"/>
+      <c r="D12" s="344"/>
+      <c r="E12" s="344" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="204"/>
-      <c r="G12" s="221"/>
-      <c r="H12" s="32" t="s">
+      <c r="F12" s="345"/>
+      <c r="G12" s="346"/>
+      <c r="H12" s="344" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32" t="s">
+      <c r="I12" s="344"/>
+      <c r="J12" s="344"/>
+      <c r="K12" s="344"/>
+      <c r="L12" s="344"/>
+      <c r="M12" s="344" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="33"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="184"/>
-      <c r="R12" s="51"/>
-      <c r="S12" s="62"/>
-      <c r="T12" s="72"/>
-      <c r="U12" s="34"/>
-      <c r="V12" s="34"/>
-      <c r="W12" s="34"/>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="241"/>
-      <c r="AA12" s="32"/>
-      <c r="AB12" s="241"/>
-      <c r="AC12" s="241"/>
-      <c r="AD12" s="32"/>
-    </row>
-    <row r="13" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="1" t="s">
+      <c r="N12" s="347"/>
+      <c r="O12" s="348"/>
+      <c r="P12" s="347"/>
+      <c r="Q12" s="349"/>
+      <c r="R12" s="350"/>
+      <c r="S12" s="351"/>
+      <c r="T12" s="352"/>
+      <c r="U12" s="353"/>
+      <c r="V12" s="353"/>
+      <c r="W12" s="353"/>
+      <c r="X12" s="344"/>
+      <c r="Y12" s="344"/>
+      <c r="Z12" s="354"/>
+      <c r="AA12" s="344"/>
+      <c r="AB12" s="354"/>
+      <c r="AC12" s="354"/>
+      <c r="AD12" s="344"/>
+    </row>
+    <row r="13" spans="1:30" s="100" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
+      <c r="B13" s="92"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="92"/>
+      <c r="E13" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="206">
+      <c r="F13" s="214">
         <v>30000</v>
       </c>
-      <c r="G13" s="223">
+      <c r="G13" s="231">
         <v>0</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="92" t="s">
         <v>188</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="356" t="s">
         <v>97</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="1" t="s">
+      <c r="J13" s="356"/>
+      <c r="K13" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="186"/>
-      <c r="R13" s="53">
+      <c r="L13" s="92"/>
+      <c r="M13" s="92"/>
+      <c r="N13" s="93"/>
+      <c r="O13" s="94"/>
+      <c r="P13" s="93"/>
+      <c r="Q13" s="357"/>
+      <c r="R13" s="95">
         <v>215</v>
       </c>
-      <c r="S13" s="64" t="s">
-        <v>186</v>
-      </c>
-      <c r="T13" s="70"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-      <c r="X13" s="10" t="s">
+      <c r="S13" s="96" t="s">
+        <v>186</v>
+      </c>
+      <c r="T13" s="97"/>
+      <c r="U13" s="98"/>
+      <c r="V13" s="98"/>
+      <c r="W13" s="98"/>
+      <c r="X13" s="98" t="s">
         <v>130</v>
       </c>
-      <c r="Y13" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z13" s="243"/>
-      <c r="AA13" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB13" s="243"/>
-      <c r="AC13" s="243" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD13" s="1" t="s">
+      <c r="Y13" s="202" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z13" s="251"/>
+      <c r="AA13" s="99" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB13" s="251"/>
+      <c r="AC13" s="251" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD13" s="92" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="101" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="1"/>
@@ -3300,7 +3401,7 @@
       </c>
     </row>
     <row r="15" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="101" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="1"/>
@@ -3357,125 +3458,125 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:30" s="111" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A16" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
+      <c r="B16" s="103"/>
+      <c r="C16" s="103"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="206">
+      <c r="F16" s="215">
         <v>30000</v>
       </c>
-      <c r="G16" s="223">
+      <c r="G16" s="232">
         <v>1</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="103" t="s">
         <v>188</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="358" t="s">
         <v>100</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="1" t="s">
+      <c r="J16" s="358"/>
+      <c r="K16" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="186"/>
-      <c r="R16" s="53">
+      <c r="L16" s="103"/>
+      <c r="M16" s="103"/>
+      <c r="N16" s="104"/>
+      <c r="O16" s="105"/>
+      <c r="P16" s="104"/>
+      <c r="Q16" s="359"/>
+      <c r="R16" s="106">
         <v>90</v>
       </c>
-      <c r="S16" s="64" t="s">
-        <v>186</v>
-      </c>
-      <c r="T16" s="70"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10" t="s">
+      <c r="S16" s="107" t="s">
+        <v>186</v>
+      </c>
+      <c r="T16" s="108"/>
+      <c r="U16" s="109"/>
+      <c r="V16" s="109"/>
+      <c r="W16" s="109"/>
+      <c r="X16" s="109" t="s">
         <v>130</v>
       </c>
-      <c r="Y16" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z16" s="243"/>
-      <c r="AA16" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB16" s="243"/>
-      <c r="AC16" s="243"/>
-      <c r="AD16" s="1" t="s">
+      <c r="Y16" s="327" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z16" s="252"/>
+      <c r="AA16" s="110" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB16" s="252"/>
+      <c r="AC16" s="252"/>
+      <c r="AD16" s="103" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2" t="s">
+      <c r="B17" s="83"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="207">
+      <c r="F17" s="216">
         <v>30000</v>
       </c>
-      <c r="G17" s="224" t="s">
+      <c r="G17" s="233" t="s">
         <v>193</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="83" t="s">
         <v>188</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="83" t="s">
         <v>200</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="83" t="s">
         <v>143</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="83" t="s">
         <v>203</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="187"/>
-      <c r="R17" s="53">
+      <c r="M17" s="83"/>
+      <c r="N17" s="84"/>
+      <c r="O17" s="85"/>
+      <c r="P17" s="84"/>
+      <c r="Q17" s="355"/>
+      <c r="R17" s="86">
         <v>105</v>
       </c>
-      <c r="S17" s="65" t="s">
-        <v>186</v>
-      </c>
-      <c r="T17" s="70"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11" t="s">
+      <c r="S17" s="87" t="s">
+        <v>186</v>
+      </c>
+      <c r="T17" s="88"/>
+      <c r="U17" s="89"/>
+      <c r="V17" s="89"/>
+      <c r="W17" s="89"/>
+      <c r="X17" s="89" t="s">
         <v>130</v>
       </c>
-      <c r="Y17" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z17" s="244"/>
-      <c r="AA17" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB17" s="244"/>
-      <c r="AC17" s="244" t="s">
+      <c r="Y17" s="201" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z17" s="253"/>
+      <c r="AA17" s="90" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB17" s="253"/>
+      <c r="AC17" s="253" t="s">
         <v>130</v>
       </c>
-      <c r="AD17" s="2" t="s">
+      <c r="AD17" s="83" t="s">
         <v>130</v>
       </c>
     </row>
@@ -12181,97 +12282,97 @@
       <c r="AC168" s="256"/>
       <c r="AD168" s="157"/>
     </row>
-    <row r="169" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A169" s="3"/>
-      <c r="B169" s="3"/>
-      <c r="C169" s="3"/>
-      <c r="D169" s="3"/>
+    <row r="169" spans="1:30" s="7" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A169" s="292"/>
+      <c r="B169" s="292"/>
+      <c r="C169" s="292"/>
+      <c r="D169" s="292"/>
       <c r="E169" s="292"/>
       <c r="F169" s="293"/>
       <c r="G169" s="294"/>
       <c r="H169" s="292"/>
-      <c r="I169" s="3"/>
-      <c r="J169" s="3"/>
-      <c r="K169" s="3"/>
-      <c r="L169" s="3"/>
-      <c r="M169" s="3"/>
-      <c r="N169" s="18"/>
-      <c r="O169" s="41"/>
-      <c r="P169" s="18"/>
-      <c r="Q169" s="188"/>
-      <c r="R169" s="55"/>
-      <c r="S169" s="66"/>
-      <c r="T169" s="70"/>
-      <c r="U169" s="12"/>
-      <c r="V169" s="12"/>
-      <c r="W169" s="12"/>
-      <c r="X169" s="12"/>
-      <c r="Y169" s="12"/>
-      <c r="Z169" s="245"/>
-      <c r="AA169" s="3"/>
-      <c r="AB169" s="245"/>
-      <c r="AC169" s="245"/>
-      <c r="AD169" s="3"/>
-    </row>
-    <row r="170" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A170" s="21" t="s">
+      <c r="I169" s="292"/>
+      <c r="J169" s="292"/>
+      <c r="K169" s="292"/>
+      <c r="L169" s="292"/>
+      <c r="M169" s="292"/>
+      <c r="N169" s="299"/>
+      <c r="O169" s="300"/>
+      <c r="P169" s="299"/>
+      <c r="Q169" s="301"/>
+      <c r="R169" s="302"/>
+      <c r="S169" s="303"/>
+      <c r="T169" s="81"/>
+      <c r="U169" s="304"/>
+      <c r="V169" s="304"/>
+      <c r="W169" s="304"/>
+      <c r="X169" s="304"/>
+      <c r="Y169" s="304"/>
+      <c r="Z169" s="305"/>
+      <c r="AA169" s="292"/>
+      <c r="AB169" s="305"/>
+      <c r="AC169" s="305"/>
+      <c r="AD169" s="292"/>
+    </row>
+    <row r="170" spans="1:30" s="285" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A170" s="315" t="s">
         <v>283</v>
       </c>
-      <c r="B170" s="21"/>
-      <c r="C170" s="21" t="s">
+      <c r="B170" s="276"/>
+      <c r="C170" s="276" t="s">
         <v>285</v>
       </c>
-      <c r="D170" s="21"/>
-      <c r="E170" s="21" t="s">
+      <c r="D170" s="276"/>
+      <c r="E170" s="276" t="s">
         <v>49</v>
       </c>
-      <c r="F170" s="218">
+      <c r="F170" s="277">
         <v>40000</v>
       </c>
-      <c r="G170" s="235">
+      <c r="G170" s="278">
         <v>0</v>
       </c>
-      <c r="H170" s="21" t="s">
+      <c r="H170" s="276" t="s">
         <v>308</v>
       </c>
-      <c r="I170" s="21" t="s">
+      <c r="I170" s="276" t="s">
         <v>197</v>
       </c>
-      <c r="J170" s="21"/>
-      <c r="K170" s="21" t="s">
+      <c r="J170" s="276"/>
+      <c r="K170" s="276" t="s">
         <v>309</v>
       </c>
-      <c r="L170" s="21"/>
-      <c r="M170" s="21"/>
-      <c r="N170" s="22"/>
-      <c r="O170" s="42"/>
-      <c r="P170" s="22"/>
-      <c r="Q170" s="194"/>
-      <c r="R170" s="53">
+      <c r="L170" s="276"/>
+      <c r="M170" s="276"/>
+      <c r="N170" s="279"/>
+      <c r="O170" s="280"/>
+      <c r="P170" s="279"/>
+      <c r="Q170" s="281"/>
+      <c r="R170" s="95">
         <f>210+1</f>
         <v>211</v>
       </c>
-      <c r="S170" s="67" t="s">
-        <v>186</v>
-      </c>
-      <c r="T170" s="70"/>
-      <c r="U170" s="23"/>
-      <c r="V170" s="23"/>
-      <c r="W170" s="23"/>
-      <c r="X170" s="23"/>
-      <c r="Y170" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z170" s="255"/>
-      <c r="AA170" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB170" s="255"/>
-      <c r="AC170" s="255"/>
-      <c r="AD170" s="21"/>
+      <c r="S170" s="282" t="s">
+        <v>186</v>
+      </c>
+      <c r="T170" s="97"/>
+      <c r="U170" s="283"/>
+      <c r="V170" s="283"/>
+      <c r="W170" s="283"/>
+      <c r="X170" s="283"/>
+      <c r="Y170" s="202" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z170" s="284"/>
+      <c r="AA170" s="202" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB170" s="284"/>
+      <c r="AC170" s="284"/>
+      <c r="AD170" s="276"/>
     </row>
     <row r="171" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A171" s="21" t="s">
+      <c r="A171" s="316" t="s">
         <v>284</v>
       </c>
       <c r="B171" s="21"/>
@@ -12330,7 +12431,7 @@
       <c r="AD171" s="21"/>
     </row>
     <row r="172" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A172" s="21" t="s">
+      <c r="A172" s="316" t="s">
         <v>286</v>
       </c>
       <c r="B172" s="21"/>
@@ -12387,119 +12488,119 @@
       </c>
       <c r="AD172" s="21"/>
     </row>
-    <row r="173" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A173" s="21" t="s">
+    <row r="173" spans="1:30" s="329" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A173" s="317" t="s">
         <v>287</v>
       </c>
-      <c r="B173" s="21"/>
-      <c r="C173" s="21" t="s">
+      <c r="B173" s="318"/>
+      <c r="C173" s="318" t="s">
         <v>285</v>
       </c>
-      <c r="D173" s="21"/>
-      <c r="E173" s="21" t="s">
+      <c r="D173" s="318"/>
+      <c r="E173" s="318" t="s">
         <v>51</v>
       </c>
-      <c r="F173" s="218">
+      <c r="F173" s="319">
         <v>40000</v>
       </c>
-      <c r="G173" s="235">
+      <c r="G173" s="320">
         <v>0</v>
       </c>
-      <c r="H173" s="21" t="s">
+      <c r="H173" s="318" t="s">
         <v>308</v>
       </c>
-      <c r="I173" s="21" t="s">
+      <c r="I173" s="318" t="s">
         <v>197</v>
       </c>
-      <c r="J173" s="21"/>
-      <c r="K173" s="21" t="s">
+      <c r="J173" s="318"/>
+      <c r="K173" s="318" t="s">
         <v>309</v>
       </c>
-      <c r="L173" s="21"/>
-      <c r="M173" s="21"/>
-      <c r="N173" s="22"/>
-      <c r="O173" s="42"/>
-      <c r="P173" s="22"/>
-      <c r="Q173" s="194"/>
-      <c r="R173" s="75">
+      <c r="L173" s="318"/>
+      <c r="M173" s="318"/>
+      <c r="N173" s="321"/>
+      <c r="O173" s="322"/>
+      <c r="P173" s="321"/>
+      <c r="Q173" s="323"/>
+      <c r="R173" s="324">
         <v>205</v>
       </c>
-      <c r="S173" s="67" t="s">
-        <v>186</v>
-      </c>
-      <c r="T173" s="70"/>
-      <c r="U173" s="23"/>
-      <c r="V173" s="23"/>
-      <c r="W173" s="23"/>
-      <c r="X173" s="23"/>
-      <c r="Y173" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z173" s="255"/>
-      <c r="AA173" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB173" s="255"/>
-      <c r="AC173" s="255" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD173" s="21"/>
+      <c r="S173" s="325" t="s">
+        <v>186</v>
+      </c>
+      <c r="T173" s="108"/>
+      <c r="U173" s="326"/>
+      <c r="V173" s="326"/>
+      <c r="W173" s="326"/>
+      <c r="X173" s="326"/>
+      <c r="Y173" s="327" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z173" s="328"/>
+      <c r="AA173" s="327" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB173" s="328"/>
+      <c r="AC173" s="328" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD173" s="318"/>
     </row>
     <row r="174" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A174" s="25" t="s">
+      <c r="A174" s="306" t="s">
         <v>288</v>
       </c>
-      <c r="B174" s="25"/>
-      <c r="C174" s="25" t="s">
+      <c r="B174" s="306"/>
+      <c r="C174" s="306" t="s">
         <v>292</v>
       </c>
-      <c r="D174" s="25"/>
-      <c r="E174" s="25" t="s">
+      <c r="D174" s="306"/>
+      <c r="E174" s="306" t="s">
         <v>49</v>
       </c>
-      <c r="F174" s="238">
+      <c r="F174" s="307">
         <v>40000</v>
       </c>
-      <c r="G174" s="239">
+      <c r="G174" s="308">
         <v>0</v>
       </c>
-      <c r="H174" s="25" t="s">
+      <c r="H174" s="306" t="s">
         <v>308</v>
       </c>
-      <c r="I174" s="25" t="s">
+      <c r="I174" s="306" t="s">
         <v>91</v>
       </c>
-      <c r="J174" s="25"/>
-      <c r="K174" s="25" t="s">
+      <c r="J174" s="306"/>
+      <c r="K174" s="306" t="s">
         <v>309</v>
       </c>
-      <c r="L174" s="25"/>
-      <c r="M174" s="25"/>
-      <c r="N174" s="26"/>
-      <c r="O174" s="43"/>
-      <c r="P174" s="26"/>
-      <c r="Q174" s="197"/>
-      <c r="R174" s="75">
+      <c r="L174" s="306"/>
+      <c r="M174" s="306"/>
+      <c r="N174" s="309"/>
+      <c r="O174" s="310"/>
+      <c r="P174" s="309"/>
+      <c r="Q174" s="311"/>
+      <c r="R174" s="133">
         <v>93</v>
       </c>
-      <c r="S174" s="68" t="s">
-        <v>186</v>
-      </c>
-      <c r="T174" s="70"/>
-      <c r="U174" s="27"/>
-      <c r="V174" s="27"/>
-      <c r="W174" s="27"/>
-      <c r="X174" s="27"/>
-      <c r="Y174" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z174" s="258"/>
-      <c r="AA174" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB174" s="258"/>
-      <c r="AC174" s="258"/>
-      <c r="AD174" s="25"/>
+      <c r="S174" s="312" t="s">
+        <v>186</v>
+      </c>
+      <c r="T174" s="88"/>
+      <c r="U174" s="313"/>
+      <c r="V174" s="313"/>
+      <c r="W174" s="313"/>
+      <c r="X174" s="313"/>
+      <c r="Y174" s="201" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z174" s="314"/>
+      <c r="AA174" s="201" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB174" s="314"/>
+      <c r="AC174" s="314"/>
+      <c r="AD174" s="306"/>
     </row>
     <row r="175" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="25" t="s">
@@ -12614,121 +12715,121 @@
       <c r="AC176" s="258"/>
       <c r="AD176" s="25"/>
     </row>
-    <row r="177" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A177" s="25" t="s">
+    <row r="177" spans="1:30" s="175" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A177" s="265" t="s">
         <v>291</v>
       </c>
-      <c r="B177" s="25"/>
-      <c r="C177" s="25" t="s">
+      <c r="B177" s="265"/>
+      <c r="C177" s="265" t="s">
         <v>292</v>
       </c>
-      <c r="D177" s="25"/>
-      <c r="E177" s="25" t="s">
+      <c r="D177" s="265"/>
+      <c r="E177" s="265" t="s">
         <v>51</v>
       </c>
-      <c r="F177" s="238">
+      <c r="F177" s="266">
         <v>40000</v>
       </c>
-      <c r="G177" s="239">
+      <c r="G177" s="267">
         <v>0</v>
       </c>
-      <c r="H177" s="25" t="s">
+      <c r="H177" s="265" t="s">
         <v>308</v>
       </c>
-      <c r="I177" s="25" t="s">
+      <c r="I177" s="265" t="s">
         <v>91</v>
       </c>
-      <c r="J177" s="25"/>
-      <c r="K177" s="25" t="s">
+      <c r="J177" s="265"/>
+      <c r="K177" s="265" t="s">
         <v>309</v>
       </c>
-      <c r="L177" s="25"/>
-      <c r="M177" s="25"/>
-      <c r="N177" s="26"/>
-      <c r="O177" s="43"/>
-      <c r="P177" s="26"/>
-      <c r="Q177" s="197"/>
-      <c r="R177" s="53">
+      <c r="L177" s="265"/>
+      <c r="M177" s="265"/>
+      <c r="N177" s="268"/>
+      <c r="O177" s="269"/>
+      <c r="P177" s="268"/>
+      <c r="Q177" s="270"/>
+      <c r="R177" s="79">
         <f>89+5</f>
         <v>94</v>
       </c>
-      <c r="S177" s="68" t="s">
-        <v>186</v>
-      </c>
-      <c r="T177" s="70"/>
-      <c r="U177" s="27"/>
-      <c r="V177" s="27"/>
-      <c r="W177" s="27"/>
-      <c r="X177" s="27"/>
-      <c r="Y177" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z177" s="258"/>
-      <c r="AA177" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB177" s="258"/>
-      <c r="AC177" s="258"/>
-      <c r="AD177" s="25"/>
-    </row>
-    <row r="178" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A178" s="21" t="s">
+      <c r="S177" s="271" t="s">
+        <v>186</v>
+      </c>
+      <c r="T177" s="81"/>
+      <c r="U177" s="272"/>
+      <c r="V177" s="272"/>
+      <c r="W177" s="272"/>
+      <c r="X177" s="272"/>
+      <c r="Y177" s="264" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z177" s="273"/>
+      <c r="AA177" s="264" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB177" s="273"/>
+      <c r="AC177" s="273"/>
+      <c r="AD177" s="265"/>
+    </row>
+    <row r="178" spans="1:30" s="285" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178" s="315" t="s">
         <v>293</v>
       </c>
-      <c r="B178" s="21"/>
-      <c r="C178" s="21" t="s">
+      <c r="B178" s="276"/>
+      <c r="C178" s="276" t="s">
         <v>294</v>
       </c>
-      <c r="D178" s="21"/>
-      <c r="E178" s="21" t="s">
+      <c r="D178" s="276"/>
+      <c r="E178" s="276" t="s">
         <v>49</v>
       </c>
-      <c r="F178" s="218">
+      <c r="F178" s="277">
         <v>40000</v>
       </c>
-      <c r="G178" s="235">
+      <c r="G178" s="278">
         <v>0</v>
       </c>
-      <c r="H178" s="21" t="s">
+      <c r="H178" s="276" t="s">
         <v>308</v>
       </c>
-      <c r="I178" s="21" t="s">
+      <c r="I178" s="276" t="s">
         <v>129</v>
       </c>
-      <c r="J178" s="21"/>
-      <c r="K178" s="21" t="s">
+      <c r="J178" s="276"/>
+      <c r="K178" s="276" t="s">
         <v>309</v>
       </c>
-      <c r="L178" s="21"/>
-      <c r="M178" s="21"/>
-      <c r="N178" s="22"/>
-      <c r="O178" s="42"/>
-      <c r="P178" s="22"/>
-      <c r="Q178" s="194"/>
-      <c r="R178" s="75">
+      <c r="L178" s="276"/>
+      <c r="M178" s="276"/>
+      <c r="N178" s="279"/>
+      <c r="O178" s="280"/>
+      <c r="P178" s="279"/>
+      <c r="Q178" s="281"/>
+      <c r="R178" s="330">
         <v>153</v>
       </c>
-      <c r="S178" s="67" t="s">
-        <v>186</v>
-      </c>
-      <c r="T178" s="70"/>
-      <c r="U178" s="23"/>
-      <c r="V178" s="23"/>
-      <c r="W178" s="23"/>
-      <c r="X178" s="23"/>
-      <c r="Y178" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z178" s="255"/>
-      <c r="AA178" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB178" s="255"/>
-      <c r="AC178" s="255"/>
-      <c r="AD178" s="21"/>
+      <c r="S178" s="282" t="s">
+        <v>186</v>
+      </c>
+      <c r="T178" s="97"/>
+      <c r="U178" s="283"/>
+      <c r="V178" s="283"/>
+      <c r="W178" s="283"/>
+      <c r="X178" s="283"/>
+      <c r="Y178" s="202" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z178" s="284"/>
+      <c r="AA178" s="202" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB178" s="284"/>
+      <c r="AC178" s="284"/>
+      <c r="AD178" s="276"/>
     </row>
     <row r="179" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A179" s="21" t="s">
+      <c r="A179" s="316" t="s">
         <v>295</v>
       </c>
       <c r="B179" s="21"/>
@@ -12785,7 +12886,7 @@
       <c r="AD179" s="21"/>
     </row>
     <row r="180" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A180" s="21" t="s">
+      <c r="A180" s="316" t="s">
         <v>296</v>
       </c>
       <c r="B180" s="21"/>
@@ -12841,118 +12942,118 @@
       <c r="AC180" s="255"/>
       <c r="AD180" s="21"/>
     </row>
-    <row r="181" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A181" s="21" t="s">
+    <row r="181" spans="1:30" s="329" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A181" s="317" t="s">
         <v>297</v>
       </c>
-      <c r="B181" s="21"/>
-      <c r="C181" s="21" t="s">
+      <c r="B181" s="318"/>
+      <c r="C181" s="318" t="s">
         <v>294</v>
       </c>
-      <c r="D181" s="21"/>
-      <c r="E181" s="21" t="s">
+      <c r="D181" s="318"/>
+      <c r="E181" s="318" t="s">
         <v>51</v>
       </c>
-      <c r="F181" s="218">
+      <c r="F181" s="319">
         <v>40000</v>
       </c>
-      <c r="G181" s="235">
+      <c r="G181" s="320">
         <v>0</v>
       </c>
-      <c r="H181" s="21" t="s">
+      <c r="H181" s="318" t="s">
         <v>308</v>
       </c>
-      <c r="I181" s="21" t="s">
+      <c r="I181" s="318" t="s">
         <v>129</v>
       </c>
-      <c r="J181" s="21"/>
-      <c r="K181" s="21" t="s">
+      <c r="J181" s="318"/>
+      <c r="K181" s="318" t="s">
         <v>309</v>
       </c>
-      <c r="L181" s="21"/>
-      <c r="M181" s="21"/>
-      <c r="N181" s="22"/>
-      <c r="O181" s="42"/>
-      <c r="P181" s="22"/>
-      <c r="Q181" s="194"/>
-      <c r="R181" s="75">
+      <c r="L181" s="318"/>
+      <c r="M181" s="318"/>
+      <c r="N181" s="321"/>
+      <c r="O181" s="322"/>
+      <c r="P181" s="321"/>
+      <c r="Q181" s="323"/>
+      <c r="R181" s="324">
         <v>153</v>
       </c>
-      <c r="S181" s="67" t="s">
-        <v>186</v>
-      </c>
-      <c r="T181" s="70"/>
-      <c r="U181" s="23"/>
-      <c r="V181" s="23"/>
-      <c r="W181" s="23"/>
-      <c r="X181" s="23"/>
-      <c r="Y181" s="295" t="s">
+      <c r="S181" s="325" t="s">
+        <v>186</v>
+      </c>
+      <c r="T181" s="108"/>
+      <c r="U181" s="326"/>
+      <c r="V181" s="326"/>
+      <c r="W181" s="326"/>
+      <c r="X181" s="326"/>
+      <c r="Y181" s="331" t="s">
         <v>217</v>
       </c>
-      <c r="Z181" s="255"/>
-      <c r="AA181" s="295" t="s">
+      <c r="Z181" s="328"/>
+      <c r="AA181" s="331" t="s">
         <v>217</v>
       </c>
-      <c r="AB181" s="255"/>
-      <c r="AC181" s="255"/>
-      <c r="AD181" s="21"/>
+      <c r="AB181" s="328"/>
+      <c r="AC181" s="328"/>
+      <c r="AD181" s="318"/>
     </row>
     <row r="182" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A182" s="25" t="s">
+      <c r="A182" s="306" t="s">
         <v>298</v>
       </c>
-      <c r="B182" s="25"/>
-      <c r="C182" s="25" t="s">
+      <c r="B182" s="306"/>
+      <c r="C182" s="306" t="s">
         <v>300</v>
       </c>
-      <c r="D182" s="25"/>
-      <c r="E182" s="25" t="s">
+      <c r="D182" s="306"/>
+      <c r="E182" s="306" t="s">
         <v>49</v>
       </c>
-      <c r="F182" s="238">
+      <c r="F182" s="307">
         <v>35000</v>
       </c>
-      <c r="G182" s="239">
+      <c r="G182" s="308">
         <v>0</v>
       </c>
-      <c r="H182" s="25" t="s">
+      <c r="H182" s="306" t="s">
         <v>308</v>
       </c>
-      <c r="I182" s="25" t="s">
+      <c r="I182" s="306" t="s">
         <v>310</v>
       </c>
-      <c r="J182" s="25"/>
-      <c r="K182" s="25" t="s">
+      <c r="J182" s="306"/>
+      <c r="K182" s="306" t="s">
         <v>309</v>
       </c>
-      <c r="L182" s="25"/>
-      <c r="M182" s="25"/>
-      <c r="N182" s="26"/>
-      <c r="O182" s="43"/>
-      <c r="P182" s="26"/>
-      <c r="Q182" s="197"/>
-      <c r="R182" s="53">
+      <c r="L182" s="306"/>
+      <c r="M182" s="306"/>
+      <c r="N182" s="309"/>
+      <c r="O182" s="310"/>
+      <c r="P182" s="309"/>
+      <c r="Q182" s="311"/>
+      <c r="R182" s="86">
         <f>165+7</f>
         <v>172</v>
       </c>
-      <c r="S182" s="68" t="s">
-        <v>186</v>
-      </c>
-      <c r="T182" s="70"/>
-      <c r="U182" s="27"/>
-      <c r="V182" s="27"/>
-      <c r="W182" s="27"/>
-      <c r="X182" s="27"/>
-      <c r="Y182" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z182" s="258"/>
-      <c r="AA182" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB182" s="258"/>
-      <c r="AC182" s="258"/>
-      <c r="AD182" s="25"/>
+      <c r="S182" s="312" t="s">
+        <v>186</v>
+      </c>
+      <c r="T182" s="88"/>
+      <c r="U182" s="313"/>
+      <c r="V182" s="313"/>
+      <c r="W182" s="313"/>
+      <c r="X182" s="313"/>
+      <c r="Y182" s="201" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z182" s="314"/>
+      <c r="AA182" s="201" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB182" s="314"/>
+      <c r="AC182" s="314"/>
+      <c r="AD182" s="306"/>
     </row>
     <row r="183" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="25" t="s">
@@ -13071,122 +13172,122 @@
       </c>
       <c r="AD184" s="25"/>
     </row>
-    <row r="185" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A185" s="25" t="s">
+    <row r="185" spans="1:30" s="175" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A185" s="265" t="s">
         <v>302</v>
       </c>
-      <c r="B185" s="25"/>
-      <c r="C185" s="25" t="s">
+      <c r="B185" s="265"/>
+      <c r="C185" s="265" t="s">
         <v>300</v>
       </c>
-      <c r="D185" s="25"/>
-      <c r="E185" s="25" t="s">
+      <c r="D185" s="265"/>
+      <c r="E185" s="265" t="s">
         <v>51</v>
       </c>
-      <c r="F185" s="238">
+      <c r="F185" s="266">
         <v>35000</v>
       </c>
-      <c r="G185" s="239">
+      <c r="G185" s="267">
         <v>0</v>
       </c>
-      <c r="H185" s="25" t="s">
+      <c r="H185" s="265" t="s">
         <v>308</v>
       </c>
-      <c r="I185" s="25" t="s">
+      <c r="I185" s="265" t="s">
         <v>310</v>
       </c>
-      <c r="J185" s="25"/>
-      <c r="K185" s="25" t="s">
+      <c r="J185" s="265"/>
+      <c r="K185" s="265" t="s">
         <v>309</v>
       </c>
-      <c r="L185" s="25"/>
-      <c r="M185" s="25"/>
-      <c r="N185" s="26"/>
-      <c r="O185" s="43"/>
-      <c r="P185" s="26"/>
-      <c r="Q185" s="197"/>
-      <c r="R185" s="53">
+      <c r="L185" s="265"/>
+      <c r="M185" s="265"/>
+      <c r="N185" s="268"/>
+      <c r="O185" s="269"/>
+      <c r="P185" s="268"/>
+      <c r="Q185" s="270"/>
+      <c r="R185" s="79">
         <f>164+2</f>
         <v>166</v>
       </c>
-      <c r="S185" s="68" t="s">
-        <v>186</v>
-      </c>
-      <c r="T185" s="70"/>
-      <c r="U185" s="27"/>
-      <c r="V185" s="27"/>
-      <c r="W185" s="27"/>
-      <c r="X185" s="27"/>
-      <c r="Y185" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z185" s="258"/>
-      <c r="AA185" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB185" s="258"/>
-      <c r="AC185" s="258"/>
-      <c r="AD185" s="25"/>
-    </row>
-    <row r="186" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A186" s="21" t="s">
+      <c r="S185" s="271" t="s">
+        <v>186</v>
+      </c>
+      <c r="T185" s="81"/>
+      <c r="U185" s="272"/>
+      <c r="V185" s="272"/>
+      <c r="W185" s="272"/>
+      <c r="X185" s="272"/>
+      <c r="Y185" s="264" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z185" s="273"/>
+      <c r="AA185" s="264" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB185" s="273"/>
+      <c r="AC185" s="273"/>
+      <c r="AD185" s="265"/>
+    </row>
+    <row r="186" spans="1:30" s="285" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186" s="315" t="s">
         <v>303</v>
       </c>
-      <c r="B186" s="21"/>
-      <c r="C186" s="21" t="s">
+      <c r="B186" s="276"/>
+      <c r="C186" s="276" t="s">
         <v>304</v>
       </c>
-      <c r="D186" s="21"/>
-      <c r="E186" s="21" t="s">
+      <c r="D186" s="276"/>
+      <c r="E186" s="276" t="s">
         <v>49</v>
       </c>
-      <c r="F186" s="218">
+      <c r="F186" s="277">
         <v>70000</v>
       </c>
-      <c r="G186" s="235">
+      <c r="G186" s="278">
         <v>0</v>
       </c>
-      <c r="H186" s="21" t="s">
+      <c r="H186" s="276" t="s">
         <v>308</v>
       </c>
-      <c r="I186" s="21" t="s">
+      <c r="I186" s="276" t="s">
         <v>91</v>
       </c>
-      <c r="J186" s="21"/>
-      <c r="K186" s="21" t="s">
+      <c r="J186" s="276"/>
+      <c r="K186" s="276" t="s">
         <v>309</v>
       </c>
-      <c r="L186" s="21"/>
-      <c r="M186" s="21"/>
-      <c r="N186" s="22"/>
-      <c r="O186" s="42"/>
-      <c r="P186" s="22"/>
-      <c r="Q186" s="194"/>
-      <c r="R186" s="53">
+      <c r="L186" s="276"/>
+      <c r="M186" s="276"/>
+      <c r="N186" s="279"/>
+      <c r="O186" s="280"/>
+      <c r="P186" s="279"/>
+      <c r="Q186" s="281"/>
+      <c r="R186" s="95">
         <f>146+3</f>
         <v>149</v>
       </c>
-      <c r="S186" s="67" t="s">
-        <v>186</v>
-      </c>
-      <c r="T186" s="70"/>
-      <c r="U186" s="23"/>
-      <c r="V186" s="23"/>
-      <c r="W186" s="23"/>
-      <c r="X186" s="23"/>
-      <c r="Y186" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z186" s="255"/>
-      <c r="AA186" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB186" s="255"/>
-      <c r="AC186" s="255"/>
-      <c r="AD186" s="21"/>
+      <c r="S186" s="282" t="s">
+        <v>186</v>
+      </c>
+      <c r="T186" s="97"/>
+      <c r="U186" s="283"/>
+      <c r="V186" s="283"/>
+      <c r="W186" s="283"/>
+      <c r="X186" s="283"/>
+      <c r="Y186" s="202" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z186" s="284"/>
+      <c r="AA186" s="202" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB186" s="284"/>
+      <c r="AC186" s="284"/>
+      <c r="AD186" s="276"/>
     </row>
     <row r="187" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A187" s="21" t="s">
+      <c r="A187" s="316" t="s">
         <v>305</v>
       </c>
       <c r="B187" s="21"/>
@@ -13244,7 +13345,7 @@
       <c r="AD187" s="21"/>
     </row>
     <row r="188" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A188" s="21" t="s">
+      <c r="A188" s="316" t="s">
         <v>306</v>
       </c>
       <c r="B188" s="21"/>
@@ -13301,124 +13402,124 @@
       </c>
       <c r="AD188" s="21"/>
     </row>
-    <row r="189" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A189" s="21" t="s">
+    <row r="189" spans="1:30" s="329" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A189" s="317" t="s">
         <v>307</v>
       </c>
-      <c r="B189" s="21"/>
-      <c r="C189" s="21" t="s">
+      <c r="B189" s="318"/>
+      <c r="C189" s="318" t="s">
         <v>304</v>
       </c>
-      <c r="D189" s="21"/>
-      <c r="E189" s="21" t="s">
+      <c r="D189" s="318"/>
+      <c r="E189" s="318" t="s">
         <v>51</v>
       </c>
-      <c r="F189" s="218">
+      <c r="F189" s="319">
         <v>70000</v>
       </c>
-      <c r="G189" s="235">
+      <c r="G189" s="320">
         <v>0</v>
       </c>
-      <c r="H189" s="21" t="s">
+      <c r="H189" s="318" t="s">
         <v>308</v>
       </c>
-      <c r="I189" s="21" t="s">
+      <c r="I189" s="318" t="s">
         <v>91</v>
       </c>
-      <c r="J189" s="21"/>
-      <c r="K189" s="21" t="s">
+      <c r="J189" s="318"/>
+      <c r="K189" s="318" t="s">
         <v>309</v>
       </c>
-      <c r="L189" s="21"/>
-      <c r="M189" s="21"/>
-      <c r="N189" s="22"/>
-      <c r="O189" s="42"/>
-      <c r="P189" s="22"/>
-      <c r="Q189" s="194"/>
-      <c r="R189" s="53">
+      <c r="L189" s="318"/>
+      <c r="M189" s="318"/>
+      <c r="N189" s="321"/>
+      <c r="O189" s="322"/>
+      <c r="P189" s="321"/>
+      <c r="Q189" s="323"/>
+      <c r="R189" s="106">
         <f>145+2</f>
         <v>147</v>
       </c>
-      <c r="S189" s="67" t="s">
-        <v>186</v>
-      </c>
-      <c r="T189" s="70"/>
-      <c r="U189" s="23"/>
-      <c r="V189" s="23"/>
-      <c r="W189" s="23"/>
-      <c r="X189" s="23"/>
-      <c r="Y189" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z189" s="255"/>
-      <c r="AA189" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB189" s="255"/>
-      <c r="AC189" s="255" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD189" s="21"/>
-    </row>
-    <row r="190" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A190" s="25" t="s">
+      <c r="S189" s="325" t="s">
+        <v>186</v>
+      </c>
+      <c r="T189" s="108"/>
+      <c r="U189" s="326"/>
+      <c r="V189" s="326"/>
+      <c r="W189" s="326"/>
+      <c r="X189" s="326"/>
+      <c r="Y189" s="327" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z189" s="328"/>
+      <c r="AA189" s="327" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB189" s="328"/>
+      <c r="AC189" s="328" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD189" s="318"/>
+    </row>
+    <row r="190" spans="1:30" s="173" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190" s="167" t="s">
         <v>311</v>
       </c>
-      <c r="B190" s="25"/>
-      <c r="C190" s="25" t="s">
+      <c r="B190" s="168"/>
+      <c r="C190" s="168" t="s">
         <v>315</v>
       </c>
-      <c r="D190" s="25"/>
-      <c r="E190" s="25" t="s">
+      <c r="D190" s="168"/>
+      <c r="E190" s="168" t="s">
         <v>49</v>
       </c>
-      <c r="F190" s="238">
+      <c r="F190" s="274">
         <v>50000</v>
       </c>
-      <c r="G190" s="239">
+      <c r="G190" s="275">
         <v>0</v>
       </c>
-      <c r="H190" s="25" t="s">
+      <c r="H190" s="168" t="s">
         <v>308</v>
       </c>
-      <c r="I190" s="25" t="s">
+      <c r="I190" s="168" t="s">
         <v>129</v>
       </c>
-      <c r="J190" s="25"/>
-      <c r="K190" s="25" t="s">
+      <c r="J190" s="168"/>
+      <c r="K190" s="168" t="s">
         <v>309</v>
       </c>
-      <c r="L190" s="25"/>
-      <c r="M190" s="25"/>
-      <c r="N190" s="26"/>
-      <c r="O190" s="43"/>
-      <c r="P190" s="26"/>
-      <c r="Q190" s="197"/>
-      <c r="R190" s="53">
+      <c r="L190" s="168"/>
+      <c r="M190" s="168"/>
+      <c r="N190" s="169"/>
+      <c r="O190" s="170"/>
+      <c r="P190" s="169"/>
+      <c r="Q190" s="196"/>
+      <c r="R190" s="95">
         <f>150+4</f>
         <v>154</v>
       </c>
-      <c r="S190" s="68" t="s">
-        <v>186</v>
-      </c>
-      <c r="T190" s="70"/>
-      <c r="U190" s="27"/>
-      <c r="V190" s="27"/>
-      <c r="W190" s="27"/>
-      <c r="X190" s="27"/>
-      <c r="Y190" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z190" s="258"/>
-      <c r="AA190" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB190" s="258"/>
-      <c r="AC190" s="258"/>
-      <c r="AD190" s="25"/>
+      <c r="S190" s="171" t="s">
+        <v>186</v>
+      </c>
+      <c r="T190" s="97"/>
+      <c r="U190" s="172"/>
+      <c r="V190" s="172"/>
+      <c r="W190" s="172"/>
+      <c r="X190" s="172"/>
+      <c r="Y190" s="202" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z190" s="257"/>
+      <c r="AA190" s="202" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB190" s="257"/>
+      <c r="AC190" s="257"/>
+      <c r="AD190" s="168"/>
     </row>
     <row r="191" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A191" s="25" t="s">
+      <c r="A191" s="174" t="s">
         <v>312</v>
       </c>
       <c r="B191" s="25"/>
@@ -13476,7 +13577,7 @@
       <c r="AD191" s="25"/>
     </row>
     <row r="192" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A192" s="25" t="s">
+      <c r="A192" s="174" t="s">
         <v>313</v>
       </c>
       <c r="B192" s="25"/>
@@ -13534,63 +13635,479 @@
       </c>
       <c r="AD192" s="25"/>
     </row>
-    <row r="193" spans="1:30" s="175" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A193" s="25" t="s">
+    <row r="193" spans="1:30" s="182" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A193" s="176" t="s">
         <v>314</v>
       </c>
-      <c r="B193" s="25"/>
-      <c r="C193" s="25" t="s">
+      <c r="B193" s="177"/>
+      <c r="C193" s="177" t="s">
         <v>315</v>
       </c>
-      <c r="D193" s="25"/>
-      <c r="E193" s="25" t="s">
+      <c r="D193" s="177"/>
+      <c r="E193" s="177" t="s">
         <v>51</v>
       </c>
-      <c r="F193" s="238">
+      <c r="F193" s="342">
         <v>50000</v>
       </c>
-      <c r="G193" s="239">
+      <c r="G193" s="343">
         <v>0</v>
       </c>
-      <c r="H193" s="25" t="s">
+      <c r="H193" s="177" t="s">
         <v>308</v>
       </c>
-      <c r="I193" s="25" t="s">
+      <c r="I193" s="177" t="s">
         <v>129</v>
       </c>
-      <c r="J193" s="25"/>
-      <c r="K193" s="25" t="s">
+      <c r="J193" s="177"/>
+      <c r="K193" s="177" t="s">
         <v>309</v>
       </c>
-      <c r="L193" s="25"/>
-      <c r="M193" s="25"/>
-      <c r="N193" s="26"/>
-      <c r="O193" s="43"/>
-      <c r="P193" s="26"/>
-      <c r="Q193" s="197"/>
-      <c r="R193" s="75">
+      <c r="L193" s="177"/>
+      <c r="M193" s="177"/>
+      <c r="N193" s="178"/>
+      <c r="O193" s="179"/>
+      <c r="P193" s="178"/>
+      <c r="Q193" s="198"/>
+      <c r="R193" s="324">
         <v>152</v>
       </c>
-      <c r="S193" s="68" t="s">
-        <v>186</v>
-      </c>
-      <c r="T193" s="70"/>
-      <c r="U193" s="27"/>
-      <c r="V193" s="27"/>
-      <c r="W193" s="27"/>
-      <c r="X193" s="27"/>
-      <c r="Y193" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z193" s="258"/>
-      <c r="AA193" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB193" s="258"/>
-      <c r="AC193" s="258" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD193" s="25"/>
+      <c r="S193" s="180" t="s">
+        <v>186</v>
+      </c>
+      <c r="T193" s="108"/>
+      <c r="U193" s="181"/>
+      <c r="V193" s="181"/>
+      <c r="W193" s="181"/>
+      <c r="X193" s="181"/>
+      <c r="Y193" s="327" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z193" s="259"/>
+      <c r="AA193" s="327" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB193" s="259"/>
+      <c r="AC193" s="259" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD193" s="177"/>
+    </row>
+    <row r="194" spans="1:30" s="7" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A194" s="113"/>
+      <c r="B194" s="113"/>
+      <c r="C194" s="113"/>
+      <c r="D194" s="113"/>
+      <c r="E194" s="113"/>
+      <c r="F194" s="217"/>
+      <c r="G194" s="234"/>
+      <c r="H194" s="113"/>
+      <c r="I194" s="113"/>
+      <c r="J194" s="113"/>
+      <c r="K194" s="113"/>
+      <c r="L194" s="113"/>
+      <c r="M194" s="113"/>
+      <c r="N194" s="114"/>
+      <c r="O194" s="115"/>
+      <c r="P194" s="114"/>
+      <c r="Q194" s="193"/>
+      <c r="R194" s="116"/>
+      <c r="S194" s="117"/>
+      <c r="T194" s="88"/>
+      <c r="U194" s="118"/>
+      <c r="V194" s="118"/>
+      <c r="W194" s="118"/>
+      <c r="X194" s="118"/>
+      <c r="Y194" s="118"/>
+      <c r="Z194" s="254"/>
+      <c r="AA194" s="113"/>
+      <c r="AB194" s="254"/>
+      <c r="AC194" s="254"/>
+      <c r="AD194" s="113"/>
+    </row>
+    <row r="195" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B195" s="1"/>
+      <c r="C195" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D195" s="1"/>
+      <c r="E195" s="276" t="s">
+        <v>49</v>
+      </c>
+      <c r="F195" s="206"/>
+      <c r="G195" s="223"/>
+      <c r="H195" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I195" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="J195" s="1"/>
+      <c r="K195" s="1"/>
+      <c r="L195" s="1"/>
+      <c r="M195" s="1"/>
+      <c r="N195" s="16"/>
+      <c r="O195" s="37"/>
+      <c r="P195" s="16"/>
+      <c r="Q195" s="186"/>
+      <c r="R195" s="56"/>
+      <c r="S195" s="64"/>
+      <c r="T195" s="70"/>
+      <c r="U195" s="10"/>
+      <c r="V195" s="10"/>
+      <c r="W195" s="10"/>
+      <c r="X195" s="10"/>
+      <c r="Y195" s="10"/>
+      <c r="Z195" s="243"/>
+      <c r="AA195" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB195" s="243"/>
+      <c r="AC195" s="243"/>
+      <c r="AD195" s="1"/>
+    </row>
+    <row r="196" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B196" s="1"/>
+      <c r="C196" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D196" s="1"/>
+      <c r="E196" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F196" s="206"/>
+      <c r="G196" s="223"/>
+      <c r="H196" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I196" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="J196" s="1"/>
+      <c r="K196" s="1"/>
+      <c r="L196" s="1"/>
+      <c r="M196" s="1"/>
+      <c r="N196" s="16"/>
+      <c r="O196" s="37"/>
+      <c r="P196" s="16"/>
+      <c r="Q196" s="186"/>
+      <c r="R196" s="56"/>
+      <c r="S196" s="64"/>
+      <c r="T196" s="70"/>
+      <c r="U196" s="10"/>
+      <c r="V196" s="10"/>
+      <c r="W196" s="10"/>
+      <c r="X196" s="10"/>
+      <c r="Y196" s="10"/>
+      <c r="Z196" s="243"/>
+      <c r="AA196" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB196" s="243"/>
+      <c r="AC196" s="243"/>
+      <c r="AD196" s="1"/>
+    </row>
+    <row r="197" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A197" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B197" s="1"/>
+      <c r="C197" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D197" s="1"/>
+      <c r="E197" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F197" s="206"/>
+      <c r="G197" s="223"/>
+      <c r="H197" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I197" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="J197" s="1"/>
+      <c r="K197" s="1"/>
+      <c r="L197" s="1"/>
+      <c r="M197" s="1"/>
+      <c r="N197" s="16"/>
+      <c r="O197" s="37"/>
+      <c r="P197" s="16"/>
+      <c r="Q197" s="186"/>
+      <c r="R197" s="56"/>
+      <c r="S197" s="64"/>
+      <c r="T197" s="70"/>
+      <c r="U197" s="10"/>
+      <c r="V197" s="10"/>
+      <c r="W197" s="10"/>
+      <c r="X197" s="10"/>
+      <c r="Y197" s="10"/>
+      <c r="Z197" s="243"/>
+      <c r="AA197" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB197" s="243"/>
+      <c r="AC197" s="243"/>
+      <c r="AD197" s="1"/>
+    </row>
+    <row r="198" spans="1:30" s="5" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A198" s="120" t="s">
+        <v>321</v>
+      </c>
+      <c r="B198" s="120"/>
+      <c r="C198" s="120" t="s">
+        <v>326</v>
+      </c>
+      <c r="D198" s="120"/>
+      <c r="E198" s="157" t="s">
+        <v>51</v>
+      </c>
+      <c r="F198" s="209"/>
+      <c r="G198" s="226"/>
+      <c r="H198" s="120" t="s">
+        <v>328</v>
+      </c>
+      <c r="I198" s="120" t="s">
+        <v>329</v>
+      </c>
+      <c r="J198" s="120"/>
+      <c r="K198" s="120"/>
+      <c r="L198" s="120"/>
+      <c r="M198" s="120"/>
+      <c r="N198" s="121"/>
+      <c r="O198" s="122"/>
+      <c r="P198" s="121"/>
+      <c r="Q198" s="189"/>
+      <c r="R198" s="154"/>
+      <c r="S198" s="124"/>
+      <c r="T198" s="81"/>
+      <c r="U198" s="125"/>
+      <c r="V198" s="125"/>
+      <c r="W198" s="125"/>
+      <c r="X198" s="125"/>
+      <c r="Y198" s="125"/>
+      <c r="Z198" s="246"/>
+      <c r="AA198" s="120" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB198" s="246"/>
+      <c r="AC198" s="246"/>
+      <c r="AD198" s="120"/>
+    </row>
+    <row r="199" spans="1:30" s="141" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A199" s="134" t="s">
+        <v>322</v>
+      </c>
+      <c r="B199" s="135"/>
+      <c r="C199" s="135" t="s">
+        <v>327</v>
+      </c>
+      <c r="D199" s="135"/>
+      <c r="E199" s="168" t="s">
+        <v>49</v>
+      </c>
+      <c r="F199" s="210"/>
+      <c r="G199" s="227"/>
+      <c r="H199" s="135" t="s">
+        <v>328</v>
+      </c>
+      <c r="I199" s="135" t="s">
+        <v>330</v>
+      </c>
+      <c r="J199" s="135"/>
+      <c r="K199" s="135"/>
+      <c r="L199" s="135"/>
+      <c r="M199" s="135"/>
+      <c r="N199" s="136"/>
+      <c r="O199" s="137"/>
+      <c r="P199" s="136"/>
+      <c r="Q199" s="190"/>
+      <c r="R199" s="138"/>
+      <c r="S199" s="139"/>
+      <c r="T199" s="97"/>
+      <c r="U199" s="140"/>
+      <c r="V199" s="140"/>
+      <c r="W199" s="140"/>
+      <c r="X199" s="140"/>
+      <c r="Y199" s="140"/>
+      <c r="Z199" s="247"/>
+      <c r="AA199" s="135" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB199" s="247"/>
+      <c r="AC199" s="247"/>
+      <c r="AD199" s="135"/>
+    </row>
+    <row r="200" spans="1:30" s="360" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A200" s="142" t="s">
+        <v>323</v>
+      </c>
+      <c r="B200" s="2"/>
+      <c r="C200" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D200" s="2"/>
+      <c r="E200" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F200" s="207"/>
+      <c r="G200" s="224"/>
+      <c r="H200" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="I200" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="J200" s="2"/>
+      <c r="K200" s="2"/>
+      <c r="L200" s="2"/>
+      <c r="M200" s="2"/>
+      <c r="N200" s="17"/>
+      <c r="O200" s="40"/>
+      <c r="P200" s="17"/>
+      <c r="Q200" s="187"/>
+      <c r="R200" s="57"/>
+      <c r="S200" s="65"/>
+      <c r="T200" s="70"/>
+      <c r="U200" s="11"/>
+      <c r="V200" s="11"/>
+      <c r="W200" s="11"/>
+      <c r="X200" s="11"/>
+      <c r="Y200" s="11"/>
+      <c r="Z200" s="244"/>
+      <c r="AA200" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB200" s="244"/>
+      <c r="AC200" s="244"/>
+      <c r="AD200" s="2"/>
+    </row>
+    <row r="201" spans="1:30" s="360" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A201" s="142" t="s">
+        <v>324</v>
+      </c>
+      <c r="B201" s="2"/>
+      <c r="C201" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D201" s="2"/>
+      <c r="E201" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F201" s="207"/>
+      <c r="G201" s="224"/>
+      <c r="H201" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="I201" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="J201" s="2"/>
+      <c r="K201" s="2"/>
+      <c r="L201" s="2"/>
+      <c r="M201" s="2"/>
+      <c r="N201" s="17"/>
+      <c r="O201" s="40"/>
+      <c r="P201" s="17"/>
+      <c r="Q201" s="187"/>
+      <c r="R201" s="57"/>
+      <c r="S201" s="65"/>
+      <c r="T201" s="70"/>
+      <c r="U201" s="11"/>
+      <c r="V201" s="11"/>
+      <c r="W201" s="11"/>
+      <c r="X201" s="11"/>
+      <c r="Y201" s="11"/>
+      <c r="Z201" s="244"/>
+      <c r="AA201" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB201" s="244"/>
+      <c r="AC201" s="244"/>
+      <c r="AD201" s="2"/>
+    </row>
+    <row r="202" spans="1:30" s="150" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A202" s="143" t="s">
+        <v>325</v>
+      </c>
+      <c r="B202" s="144"/>
+      <c r="C202" s="144" t="s">
+        <v>327</v>
+      </c>
+      <c r="D202" s="144"/>
+      <c r="E202" s="177" t="s">
+        <v>51</v>
+      </c>
+      <c r="F202" s="211"/>
+      <c r="G202" s="228"/>
+      <c r="H202" s="144" t="s">
+        <v>328</v>
+      </c>
+      <c r="I202" s="144" t="s">
+        <v>330</v>
+      </c>
+      <c r="J202" s="144"/>
+      <c r="K202" s="144"/>
+      <c r="L202" s="144"/>
+      <c r="M202" s="144"/>
+      <c r="N202" s="145"/>
+      <c r="O202" s="146"/>
+      <c r="P202" s="145"/>
+      <c r="Q202" s="191"/>
+      <c r="R202" s="156"/>
+      <c r="S202" s="148"/>
+      <c r="T202" s="108"/>
+      <c r="U202" s="149"/>
+      <c r="V202" s="149"/>
+      <c r="W202" s="149"/>
+      <c r="X202" s="149"/>
+      <c r="Y202" s="149"/>
+      <c r="Z202" s="248"/>
+      <c r="AA202" s="144" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB202" s="248"/>
+      <c r="AC202" s="248"/>
+      <c r="AD202" s="144"/>
+    </row>
+    <row r="203" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="A203" s="332"/>
+      <c r="B203" s="332"/>
+      <c r="C203" s="332"/>
+      <c r="D203" s="332"/>
+      <c r="E203" s="332"/>
+      <c r="F203" s="333"/>
+      <c r="G203" s="334"/>
+      <c r="H203" s="332"/>
+      <c r="I203" s="332"/>
+      <c r="J203" s="332"/>
+      <c r="K203" s="332"/>
+      <c r="L203" s="332"/>
+      <c r="M203" s="332"/>
+      <c r="N203" s="335"/>
+      <c r="O203" s="336"/>
+      <c r="P203" s="335"/>
+      <c r="Q203" s="337"/>
+      <c r="R203" s="338"/>
+      <c r="S203" s="339"/>
+      <c r="T203" s="88"/>
+      <c r="U203" s="340"/>
+      <c r="V203" s="340"/>
+      <c r="W203" s="340"/>
+      <c r="X203" s="340"/>
+      <c r="Y203" s="340"/>
+      <c r="Z203" s="341"/>
+      <c r="AA203" s="332"/>
+      <c r="AB203" s="341"/>
+      <c r="AC203" s="341"/>
+      <c r="AD203" s="332"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
finished plots for doping chapter
</commit_message>
<xml_diff>
--- a/ProbenSpreadsheet.xlsx
+++ b/ProbenSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdcj\Documents\_user\_MasterThesis\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E60F24A-785B-4CF0-BD04-CF800886414B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CA3D01-D18B-4483-9608-E68B402EFF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51720" yWindow="4785" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51720" yWindow="7155" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Probenübersicht" sheetId="1" r:id="rId1"/>
@@ -2774,9 +2774,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF206"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J91" sqref="J91"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L93" sqref="L93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
finished strain analysis of fluence variation samples
</commit_message>
<xml_diff>
--- a/ProbenSpreadsheet.xlsx
+++ b/ProbenSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdcj\Documents\_user\_MasterThesis\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CA3D01-D18B-4483-9608-E68B402EFF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F182EFA6-7C1E-4925-A95F-66C35C5FF51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51720" yWindow="7155" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Probenübersicht" sheetId="1" r:id="rId1"/>
@@ -2774,9 +2774,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF206"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L93" sqref="L93"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA134" sqref="AA134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
added some misc. plots
</commit_message>
<xml_diff>
--- a/ProbenSpreadsheet.xlsx
+++ b/ProbenSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdcj\Documents\_user\_MasterThesis\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F182EFA6-7C1E-4925-A95F-66C35C5FF51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC11487-A8F5-464B-A118-DA1208941ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2775,8 +2775,8 @@
   <dimension ref="A1:AF206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA134" sqref="AA134"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I141" sqref="I141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -12353,7 +12353,7 @@
       <c r="AD162" s="257"/>
       <c r="AE162" s="257"/>
       <c r="AF162" s="25" t="s">
-        <v>215</v>
+        <v>130</v>
       </c>
     </row>
     <row r="163" spans="1:32" s="174" customFormat="1" x14ac:dyDescent="0.55000000000000004">

</xml_diff>